<commit_message>
Fix bugs. Added more unit tests
</commit_message>
<xml_diff>
--- a/src/test/resources/FMEA.xlsx
+++ b/src/test/resources/FMEA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/zendrahealth/excel-validator/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B4BF3A-4D05-B14C-BBFA-7508FFFEB0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CD8BAA-68C2-DC41-A37F-50327F990E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="900" windowWidth="32120" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMEA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="140">
   <si>
     <t>Item</t>
   </si>
@@ -1603,10 +1603,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1804,7 +1804,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="66"/>
       <c r="B3" s="30" t="s">
         <v>17</v>
@@ -1872,7 +1872,10 @@
       <c r="U3" s="32">
         <v>2</v>
       </c>
-      <c r="V3" s="32"/>
+      <c r="V3" s="32">
+        <f>T3*U3</f>
+        <v>4</v>
+      </c>
       <c r="W3" s="32">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -2027,7 +2030,10 @@
       <c r="U5" s="32">
         <v>2</v>
       </c>
-      <c r="V5" s="32"/>
+      <c r="V5" s="32">
+        <f>T5*U5</f>
+        <v>4</v>
+      </c>
       <c r="W5" s="32">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -2109,7 +2115,10 @@
       <c r="U6" s="32">
         <v>1</v>
       </c>
-      <c r="V6" s="32"/>
+      <c r="V6" s="32">
+        <f>T6*U6</f>
+        <v>1</v>
+      </c>
       <c r="W6" s="32">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -2123,7 +2132,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="66"/>
       <c r="B7" s="30" t="s">
         <v>29</v>
@@ -2191,7 +2200,10 @@
       <c r="U7" s="32">
         <v>2</v>
       </c>
-      <c r="V7" s="32"/>
+      <c r="V7" s="32">
+        <f>T7*U7</f>
+        <v>2</v>
+      </c>
       <c r="W7" s="32">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -2205,7 +2217,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="66"/>
       <c r="B8" s="30" t="s">
         <v>30</v>
@@ -2288,7 +2300,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="112" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="66"/>
       <c r="B9" s="30" t="s">
         <v>31</v>
@@ -2371,7 +2383,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="66"/>
       <c r="B10" s="30" t="s">
         <v>79</v>
@@ -2398,6 +2410,7 @@
 Identity theft, Exploitation: Ransom or Targeting</v>
       </c>
       <c r="I10" s="27">
+        <f>VLOOKUP(VLOOKUP($G10,'Accidents, Hazards &amp; Harms '!$H$2:$I$166,2,FALSE),'Accidents, Hazards &amp; Harms '!$K$2:$M$135,3,FALSE)</f>
         <v>2</v>
       </c>
       <c r="J10" s="30">
@@ -2421,8 +2434,9 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="P10" s="28" t="s">
-        <v>43</v>
+      <c r="P10" s="33" t="str">
+        <f t="array" ref="P10">INDEX('Scoring criteria'!$H$4:$L$6, MATCH(FMEA!N10, 'Scoring criteria'!$F$4:$F$6, 0), MATCH(FMEA!I10, 'Scoring criteria'!$H$3:$L$3, 0))</f>
+        <v>B</v>
       </c>
       <c r="Q10" s="35" t="s">
         <v>132</v>
@@ -2454,6 +2468,12 @@
       <c r="Y10" s="33" t="str">
         <f t="array" ref="Y10">INDEX('Scoring criteria'!$H$4:$L$6, MATCH(FMEA!W10, 'Scoring criteria'!$F$4:$F$6, 0), MATCH(FMEA!S10, 'Scoring criteria'!$H$3:$L$3, 0))</f>
         <v>A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V11" s="32">
+        <f>T11*U11</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2465,17 +2485,17 @@
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="D7:D9"/>
   </mergeCells>
-  <conditionalFormatting sqref="P1:P10 Y4:Y10">
+  <conditionalFormatting sqref="Y4:Y10 P1:P10">
     <cfRule type="cellIs" dxfId="37" priority="73" operator="equal">
       <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P10 Y4:Y10">
+  <conditionalFormatting sqref="Y4:Y10 P1:P10">
     <cfRule type="cellIs" dxfId="36" priority="74" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P10 Y4:Y10">
+  <conditionalFormatting sqref="Y4:Y10 P1:P10">
     <cfRule type="cellIs" dxfId="35" priority="75" operator="equal">
       <formula>"A"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updates for initial risk assessment formula column F to '=VLOOKUP(E<rowIndex>,'Accidents, Hazards & Harms 'statusB:90,2,FALSE)'
</commit_message>
<xml_diff>
--- a/src/test/resources/FMEA.xlsx
+++ b/src/test/resources/FMEA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/zendrahealth/excel-validator/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CD8BAA-68C2-DC41-A37F-50327F990E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7E571D-8239-284D-8153-9847A8725936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="900" windowWidth="32120" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="500" windowWidth="32120" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMEA" sheetId="1" r:id="rId1"/>
@@ -1605,8 +1605,8 @@
   </sheetPr>
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1732,7 +1732,7 @@
         <v>130</v>
       </c>
       <c r="F2" s="27" t="str">
-        <f>VLOOKUP(E2,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E2,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G2" s="27" t="str">
@@ -1788,11 +1788,11 @@
         <v>2</v>
       </c>
       <c r="V2" s="32">
-        <f>T2*U2</f>
+        <f t="shared" ref="V2:V7" si="3">T2*U2</f>
         <v>4</v>
       </c>
       <c r="W2" s="32">
-        <f t="shared" ref="W2:W7" si="3">IF(V2&lt;16, IF(V2&lt;8, 1, 2), 3)</f>
+        <f t="shared" ref="W2:W7" si="4">IF(V2&lt;16, IF(V2&lt;8, 1, 2), 3)</f>
         <v>1</v>
       </c>
       <c r="X2" s="32">
@@ -1817,7 +1817,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="27" t="str">
-        <f>VLOOKUP(E3,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E3,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G3" s="27" t="str">
@@ -1873,15 +1873,15 @@
         <v>2</v>
       </c>
       <c r="V3" s="32">
-        <f>T3*U3</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="W3" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X3" s="32">
-        <f t="shared" ref="X3:X7" si="4">S3*T3*U3</f>
+        <f t="shared" ref="X3:X7" si="5">S3*T3*U3</f>
         <v>8</v>
       </c>
       <c r="Y3" s="33" t="str">
@@ -1900,7 +1900,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="27" t="str">
-        <f>VLOOKUP(E4,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E4,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G4" s="27" t="str">
@@ -1952,15 +1952,15 @@
         <v>2</v>
       </c>
       <c r="V4" s="32">
-        <f>T4*U4</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="W4" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X4" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="Y4" s="33" t="str">
@@ -1979,7 +1979,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="27" t="str">
-        <f>VLOOKUP(E5,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E5,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G5" s="27" t="str">
@@ -2031,15 +2031,15 @@
         <v>2</v>
       </c>
       <c r="V5" s="32">
-        <f>T5*U5</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="W5" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X5" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="Y5" s="33" t="str">
@@ -2060,7 +2060,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="27" t="str">
-        <f>VLOOKUP(E6,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E6,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G6" s="27" t="str">
@@ -2116,15 +2116,15 @@
         <v>1</v>
       </c>
       <c r="V6" s="32">
-        <f>T6*U6</f>
-        <v>1</v>
-      </c>
-      <c r="W6" s="32">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="W6" s="32">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="X6" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="Y6" s="33" t="str">
@@ -2145,7 +2145,7 @@
         <v>28</v>
       </c>
       <c r="F7" s="27" t="str">
-        <f>VLOOKUP(E7,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E7,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G7" s="27" t="str">
@@ -2201,15 +2201,15 @@
         <v>2</v>
       </c>
       <c r="V7" s="32">
-        <f>T7*U7</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W7" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="X7" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="Y7" s="33" t="str">
@@ -2228,7 +2228,7 @@
         <v>91</v>
       </c>
       <c r="F8" s="27" t="str">
-        <f>VLOOKUP(E8,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E8,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G8" s="27" t="str">
@@ -2257,7 +2257,7 @@
         <v>8</v>
       </c>
       <c r="N8" s="32">
-        <f t="shared" ref="N8:N10" si="5">IF(M8&lt;16, IF(M8&lt;8, 1, 2), 3)</f>
+        <f t="shared" ref="N8:N10" si="6">IF(M8&lt;16, IF(M8&lt;8, 1, 2), 3)</f>
         <v>2</v>
       </c>
       <c r="O8" s="32">
@@ -2284,15 +2284,15 @@
         <v>1</v>
       </c>
       <c r="V8" s="32">
-        <f t="shared" ref="V8:V10" si="6">T8*U8</f>
+        <f t="shared" ref="V8:V10" si="7">T8*U8</f>
         <v>1</v>
       </c>
       <c r="W8" s="32">
-        <f t="shared" ref="W8:W10" si="7">IF(V8&lt;16, IF(V8&lt;8, 1, 2), 3)</f>
+        <f t="shared" ref="W8:W10" si="8">IF(V8&lt;16, IF(V8&lt;8, 1, 2), 3)</f>
         <v>1</v>
       </c>
       <c r="X8" s="32">
-        <f t="shared" ref="X8:X10" si="8">S8*T8*U8</f>
+        <f t="shared" ref="X8:X10" si="9">S8*T8*U8</f>
         <v>2</v>
       </c>
       <c r="Y8" s="33" t="str">
@@ -2311,7 +2311,7 @@
         <v>92</v>
       </c>
       <c r="F9" s="27" t="str">
-        <f>VLOOKUP(E9,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E9,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ03</v>
       </c>
       <c r="G9" s="27" t="str">
@@ -2340,7 +2340,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O9" s="32">
@@ -2367,15 +2367,15 @@
         <v>1</v>
       </c>
       <c r="V9" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="W9" s="32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="X9" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="Y9" s="33" t="str">
@@ -2396,7 +2396,7 @@
         <v>128</v>
       </c>
       <c r="F10" s="27" t="str">
-        <f>VLOOKUP(E10,'Accidents, Hazards &amp; Harms '!$B$2:$C$120,2,FALSE)</f>
+        <f>VLOOKUP(E10,'Accidents, Hazards &amp; Harms '!$B$2:$C$190,2,FALSE)</f>
         <v>HAZ10</v>
       </c>
       <c r="G10" s="27" t="str">
@@ -2427,7 +2427,7 @@
         <v>8</v>
       </c>
       <c r="N10" s="32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O10" s="32">
@@ -2454,15 +2454,15 @@
         <v>1</v>
       </c>
       <c r="V10" s="32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="W10" s="32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="X10" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="Y10" s="33" t="str">

</xml_diff>